<commit_message>
Changed Gantt and Sales Data
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Task Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Pat</t>
   </si>
   <si>
-    <t>Gantt Chart</t>
-  </si>
-  <si>
     <t>Create Website</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Wednesday 04/11/15</t>
   </si>
   <si>
-    <t>30 Mins</t>
-  </si>
-  <si>
     <t>Roles</t>
   </si>
   <si>
@@ -115,6 +109,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Finishing Touches</t>
   </si>
 </sst>
 </file>
@@ -130,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,13 +136,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,8 +205,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,12 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,254 +536,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="6"/>
+    </row>
+    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="1" t="s">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="1" t="s">
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="6"/>
+    </row>
+    <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="3"/>
-    </row>
-    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="3"/>
-    </row>
-    <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.40277777777777801</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.40972222222222199</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.43055555555555503</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.121527777777778</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0.12847222222222199</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0.13541666666666699</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.48263888888888901</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0.49652777777777801</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0.50347222222222199</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0.52430555555555503</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="AG3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.38194444444444442</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.40277777777777801</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.40972222222222199</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.42361111111111099</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0.43055555555555503</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0.4375</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0.44444444444444398</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0.10069444444444443</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0.1076388888888889</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0.114583333333333</v>
-      </c>
-      <c r="R3" s="4">
-        <v>0.121527777777778</v>
-      </c>
-      <c r="S3" s="4">
-        <v>0.12847222222222199</v>
-      </c>
-      <c r="T3" s="4">
-        <v>0.13541666666666699</v>
-      </c>
-      <c r="U3" s="4">
-        <v>0.46180555555555558</v>
-      </c>
-      <c r="V3" s="4">
-        <v>0.46875</v>
-      </c>
-      <c r="W3" s="4">
-        <v>0.47569444444444398</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0.48263888888888901</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>0.48958333333333298</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>0.49652777777777801</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>0.50347222222222199</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>0.51041666666666696</v>
-      </c>
-      <c r="AC3" s="4">
-        <v>0.51736111111111105</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>0.52430555555555503</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>0.53125</v>
-      </c>
-      <c r="AG3" s="6"/>
-    </row>
-    <row r="4" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="8"/>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="G9" s="8"/>
+      <c r="D9" s="3"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -804,116 +794,108 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="9"/>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+    </row>
+    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-    </row>
-    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Changed Gantt Chart and Sales data
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Task Name</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Roles</t>
   </si>
   <si>
-    <t>50 Mins</t>
-  </si>
-  <si>
     <t>10 Mins</t>
   </si>
   <si>
@@ -112,13 +109,40 @@
   </si>
   <si>
     <t>Finishing Touches</t>
+  </si>
+  <si>
+    <t>Predecessor</t>
+  </si>
+  <si>
+    <t>Gantt Chart 28/10 - 4/11</t>
+  </si>
+  <si>
+    <t>60 Mins</t>
+  </si>
+  <si>
+    <t>Sean/Matt</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t>90 Mins</t>
+  </si>
+  <si>
+    <t>140 Mins</t>
+  </si>
+  <si>
+    <t>All Events</t>
+  </si>
+  <si>
+    <t>Start Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +150,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,8 +179,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -201,13 +246,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -219,7 +326,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +642,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,383 +650,714 @@
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="1:33" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="4" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="4" t="s">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="5"/>
     </row>
     <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="4" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="4" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="4" t="s">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="4" t="s">
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="6"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="9">
         <v>0.375</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="10">
         <v>0.38194444444444442</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="10">
         <v>0.3888888888888889</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="10">
         <v>0.39583333333333298</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="10">
         <v>0.40277777777777801</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="10">
         <v>0.40972222222222199</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="10">
         <v>0.41666666666666702</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="10">
         <v>0.42361111111111099</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="10">
         <v>0.43055555555555503</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="10">
         <v>0.4375</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="10">
         <v>0.44444444444444398</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="10">
         <v>0.10069444444444443</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="10">
         <v>0.1076388888888889</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="10">
         <v>0.114583333333333</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="10">
         <v>0.121527777777778</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="10">
         <v>0.12847222222222199</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="10">
         <v>0.13541666666666699</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="10">
         <v>0.46180555555555558</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="10">
         <v>0.46875</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="10">
         <v>0.47569444444444398</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Y3" s="10">
         <v>0.48263888888888901</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Z3" s="10">
         <v>0.48958333333333298</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="10">
         <v>0.49652777777777801</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AB3" s="10">
         <v>0.50347222222222199</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AC3" s="10">
         <v>0.51041666666666696</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="10">
         <v>0.51736111111111105</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AE3" s="10">
         <v>0.52430555555555503</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AF3" s="10">
         <v>0.53125</v>
       </c>
-      <c r="AG3" s="3"/>
+      <c r="AG3" s="2"/>
     </row>
     <row r="4" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+    </row>
+    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>A4</f>
+        <v>Assign Roles</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+    </row>
+    <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>A4</f>
+        <v>Assign Roles</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f>A6</f>
+        <v>Add Collaberators</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+    </row>
+    <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>A6</f>
+        <v>Add Collaberators</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+    </row>
+    <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>A7</f>
+        <v>Plan Website Design</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="12"/>
+      <c r="AF9" s="12"/>
+    </row>
+    <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>A9</f>
+        <v>Create Website</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="12"/>
+    </row>
+    <row r="11" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>A6</f>
+        <v>Add Collaberators</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+    </row>
+    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>A11</f>
+        <v>Design Brochure</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+    </row>
+    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f>A8</f>
+        <v>Enter Data on SpreadSheet</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+    </row>
+    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>A13</f>
+        <v>Design C# Program</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+    </row>
+    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-    </row>
-    <row r="11" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-    </row>
-    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-    </row>
-    <row r="15" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="U2:Y2"/>
-    <mergeCell ref="Z2:AE2"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="U1:AE1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="E1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AF1"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>